<commit_message>
complete and send documents to Justin
</commit_message>
<xml_diff>
--- a/nutrition wellshop estimation.xlsx
+++ b/nutrition wellshop estimation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,12 +11,12 @@
     <sheet name="FRONTEND-APPS" sheetId="2" r:id="rId2"/>
     <sheet name="QA" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
   <si>
     <t>Setup user information ( admin, HDT, trainer, clients)</t>
   </si>
@@ -259,12 +259,36 @@
   <si>
     <t>Repoting methods</t>
   </si>
+  <si>
+    <t>Working Time (8 hours/day)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Backend</t>
+  </si>
+  <si>
+    <t>(Security Configuration)</t>
+  </si>
+  <si>
+    <t>Total Front-end</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Working Time (per hour)</t>
+  </si>
+  <si>
+    <t>Cost(12$/hour)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +329,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -404,6 +446,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,6 +478,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -428,9 +502,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,6 +591,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -554,6 +626,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -729,35 +802,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:C29"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="3" max="4" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="39" x14ac:dyDescent="0.6">
+      <c r="A1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
@@ -765,288 +843,557 @@
         <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="2">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2">
+        <f>C5*12</f>
+        <v>480</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="2">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ref="D6:D23" si="0">C6*12</f>
+        <v>144</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="2">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" s="2">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" s="2">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" s="2">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" s="2">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" s="2">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18" s="2">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19" s="2">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" s="2">
+        <v>14</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21" s="2">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="C22" s="2">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="15" t="s">
+      <c r="C23" s="2">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="17">
+        <f>SUM(C5:C23)</f>
+        <v>224</v>
+      </c>
+      <c r="D24" s="17">
+        <f>SUM(D5:D23)</f>
+        <v>2688</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="C26" s="2">
+        <v>14</v>
+      </c>
+      <c r="D26" s="2">
+        <f>C26*12</f>
+        <v>168</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3">
+        <v>21</v>
+      </c>
+      <c r="C27" s="2">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D29" si="1">C27*12</f>
+        <v>96</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="2">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="22" t="s">
+      <c r="C29" s="2">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="17">
+        <f>SUM(C26:C29)</f>
+        <v>38</v>
+      </c>
+      <c r="D30" s="17">
+        <f>SUM(D26:D29)</f>
+        <v>456</v>
+      </c>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>1</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C32" s="5">
+        <v>8</v>
+      </c>
+      <c r="D32" s="5">
+        <f>C32*12</f>
+        <v>96</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>2</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C33" s="5">
+        <v>8</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" ref="D33:D35" si="2">C33*12</f>
+        <v>96</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <v>3</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="5">
+      <c r="C34" s="5">
+        <v>8</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>4</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="5">
+      <c r="C35" s="5">
+        <v>8</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
         <v>4</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
+      <c r="C36" s="5">
+        <v>40</v>
+      </c>
+      <c r="D36" s="5">
+        <f>C36*12</f>
+        <v>480</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="17">
+        <f>SUM(C32:C36)</f>
+        <v>72</v>
+      </c>
+      <c r="D37" s="17">
+        <f>SUM(D32:D36)</f>
+        <v>864</v>
+      </c>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="25"/>
+      <c r="C38" s="21">
+        <f>SUM(C24,C30,C37)</f>
+        <v>334</v>
+      </c>
+      <c r="D38" s="21">
+        <f>SUM(D24,D30,D37)</f>
+        <v>4008</v>
+      </c>
+      <c r="E38" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A4:C4"/>
+  <mergeCells count="7">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1054,29 +1401,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="39" x14ac:dyDescent="0.6">
+      <c r="A1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -1084,261 +1435,484 @@
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <f>C4*12</f>
+        <v>96</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" ref="D5:D11" si="0">C5*12</f>
+        <v>96</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="2">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>288</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="2">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="15" t="s">
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="17">
+        <f>SUM(C4:C11)</f>
+        <v>88</v>
+      </c>
+      <c r="D12" s="17">
+        <f>SUM(D4:D11)</f>
+        <v>1056</v>
+      </c>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="2">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <f>C14*12</f>
+        <v>96</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" ref="D15:D23" si="1">C15*12</f>
+        <v>96</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2">
+      <c r="C16" s="2">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="2">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2">
+      <c r="C18" s="2">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2">
+      <c r="C19" s="2">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>7</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2">
-        <v>8</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2">
+      <c r="C21" s="5">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>9</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90">
-      <c r="A22" s="2">
+    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>10</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="6">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="21" t="s">
+    <row r="24" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="19">
+        <f>SUM(C14:C23)</f>
+        <v>86</v>
+      </c>
+      <c r="D24" s="19">
+        <f>SUM(D14:D23)</f>
+        <v>1032</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2">
+      <c r="C26" s="2">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2">
+        <f>C26*12</f>
+        <v>96</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>2</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2">
+      <c r="C27" s="2">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D28" si="2">C27*12</f>
+        <v>96</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>3</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C28" s="2">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="17">
+        <f>SUM(C26:C28)</f>
+        <v>24</v>
+      </c>
+      <c r="D29" s="17">
+        <f>SUM(D26:D28)</f>
+        <v>288</v>
+      </c>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="16">
+        <f>SUM(C12,C24,C29)</f>
+        <v>198</v>
+      </c>
+      <c r="D30" s="16">
+        <f>SUM(D12,D24,D29)</f>
+        <v>2376</v>
+      </c>
+      <c r="E30" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A23:C23"/>
+  <mergeCells count="8">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
     <col min="3" max="3" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>47</v>
       </c>
@@ -1349,7 +1923,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
+    <row r="2" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1358,7 +1932,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="48" customHeight="1">
+    <row r="3" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1367,7 +1941,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="48" customHeight="1">
+    <row r="4" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1376,7 +1950,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="48" customHeight="1">
+    <row r="5" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1385,7 +1959,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="48" customHeight="1">
+    <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1394,7 +1968,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" ht="48" customHeight="1">
+    <row r="7" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1403,7 +1977,7 @@
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="48" customHeight="1">
+    <row r="8" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1412,7 +1986,7 @@
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>

</xml_diff>